<commit_message>
added smtp server and port to get email sending
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b9e42cbdc657b05/Desktop/Python Codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b9e42cbdc657b05/Desktop/Python Codes/automated emails/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{96577C8C-6F30-4079-8D33-8BDF37B3ADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="5424" windowWidth="21624" windowHeight="11244" xr2:uid="{35C39BFD-5A17-46F4-A9B3-59F61B99286A}"/>
+    <workbookView xWindow="1416" yWindow="1716" windowWidth="21624" windowHeight="11244" xr2:uid="{35C39BFD-5A17-46F4-A9B3-59F61B99286A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>